<commit_message>
Update the support for semantic translation (only supporting  some simple assignment statement now). For the convenience of the coding, temporally remove the return of results
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,11 +605,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>a</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20">
@@ -787,11 +787,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>+</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34">
@@ -800,11 +800,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>61</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35">
@@ -813,11 +813,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>*</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>80</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36">
@@ -826,11 +826,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>35</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37">
@@ -839,7 +839,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -852,11 +852,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>+</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>62</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39">
@@ -865,11 +865,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>4</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40">
@@ -878,11 +878,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="41">
@@ -891,11 +891,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>e</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42">
@@ -904,11 +904,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>=</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43">
@@ -917,7 +917,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -930,11 +930,206 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>)</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="C46" t="n">
         <v>62</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>f</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>(</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>(</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>*</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>)</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update the support for if statement
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C70"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -735,11 +735,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>d</t>
+          <t xml:space="preserve">	d</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>81</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30">
@@ -1272,6 +1272,330 @@
         </is>
       </c>
       <c r="C70" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>&lt;</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <f>=</f>
+        <v/>
+      </c>
+      <c r="C90" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update the support for if statement and while statement
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1281,11 +1281,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>while</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>17</v>
+        <v>29</v>
       </c>
     </row>
     <row r="72">
@@ -1596,6 +1596,213 @@
         </is>
       </c>
       <c r="C95" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <f>=</f>
+        <v/>
+      </c>
+      <c r="C98" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>if</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>&gt;=</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>:</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	while</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>#</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>=</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
         <v>80</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Version 1.0 Update the indent detection
</commit_message>
<xml_diff>
--- a/result.xlsx
+++ b/result.xlsx
@@ -7,7 +7,7 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Word-code" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C111"/>
+  <dimension ref="A1:C110"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -384,11 +384,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>def</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>81</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3">
@@ -397,11 +397,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>getAllWordCode</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
@@ -423,11 +423,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>self</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>80</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -436,11 +436,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>,</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7">
@@ -449,11 +449,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>data_list</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
@@ -462,11 +462,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9">
@@ -475,11 +475,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>:</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>61</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10">
@@ -488,7 +488,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>variable</t>
+          <t>word_code_list</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -501,11 +501,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>=</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12">
@@ -514,11 +514,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>[</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13">
@@ -527,11 +527,11 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>]</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
@@ -540,11 +540,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>for</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
@@ -553,7 +553,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>sentence</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -566,11 +566,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>in</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>46</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17">
@@ -579,11 +579,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>data_list</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18">
@@ -592,11 +592,11 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>:</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19">
@@ -605,11 +605,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>#</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20">
@@ -618,11 +618,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>c</t>
+          <t>print</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>81</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21">
@@ -631,11 +631,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>46</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22">
@@ -644,11 +644,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>sentence</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23">
@@ -657,11 +657,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>35</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24">
@@ -670,11 +670,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>sen_list</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25">
@@ -683,11 +683,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>=</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="26">
@@ -696,11 +696,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>sentence</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27">
@@ -709,11 +709,11 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28">
@@ -722,11 +722,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>split</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29">
@@ -735,11 +735,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t xml:space="preserve">		d</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>-1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30">
@@ -748,11 +748,11 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>'</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="31">
@@ -761,11 +761,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>'</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32">
@@ -774,11 +774,11 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="33">
@@ -787,11 +787,11 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>#</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34">
@@ -800,11 +800,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>print</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35">
@@ -813,11 +813,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36">
@@ -826,11 +826,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>sen_list</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37">
@@ -839,11 +839,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38">
@@ -852,11 +852,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>#</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39">
@@ -865,11 +865,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>print</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40">
@@ -878,11 +878,11 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41">
@@ -891,7 +891,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>sen_list</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -904,11 +904,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="43">
@@ -917,11 +917,11 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>tmp_list_origin</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44">
@@ -930,11 +930,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>=</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="45">
@@ -943,11 +943,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>[</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>80</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46">
@@ -956,11 +956,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>]</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47">
@@ -969,7 +969,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>f</t>
+          <t>tmp_list_dict</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -995,11 +995,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>[</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50">
@@ -1008,11 +1008,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>]</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51">
@@ -1021,11 +1021,11 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>for</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>37</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52">
@@ -1034,11 +1034,11 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53">
@@ -1047,11 +1047,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>in</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>37</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54">
@@ -1060,11 +1060,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>(</t>
+          <t>sen_list</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>61</v>
+        <v>81</v>
       </c>
     </row>
     <row r="55">
@@ -1073,11 +1073,11 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>:</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>80</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56">
@@ -1086,11 +1086,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>*</t>
+          <t>#</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="57">
@@ -1099,11 +1099,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>print</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="58">
@@ -1112,11 +1112,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>)</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59">
@@ -1125,11 +1125,11 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>43</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60">
@@ -1138,11 +1138,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>g</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="61">
@@ -1151,11 +1151,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>tmp_list_origin</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62">
@@ -1164,11 +1164,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="63">
@@ -1177,11 +1177,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>extend</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="64">
@@ -1190,11 +1190,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65">
@@ -1203,11 +1203,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>self</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
@@ -1216,11 +1216,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="67">
@@ -1229,11 +1229,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>__stringProcessing</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68">
@@ -1242,11 +1242,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69">
@@ -1255,11 +1255,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>35</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70">
@@ -1268,11 +1268,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>80</v>
+        <v>62</v>
       </c>
     </row>
     <row r="71">
@@ -1281,11 +1281,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>while</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>29</v>
+        <v>62</v>
       </c>
     </row>
     <row r="72">
@@ -1294,11 +1294,11 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>#</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>81</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73">
@@ -1307,11 +1307,11 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>&lt;</t>
+          <t>print</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>48</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74">
@@ -1320,11 +1320,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75">
@@ -1333,11 +1333,11 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>and</t>
+          <t>tmp_list_origin</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>69</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76">
@@ -1346,11 +1346,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="77">
@@ -1359,11 +1359,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>&lt;</t>
+          <t>for</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>48</v>
+        <v>13</v>
       </c>
     </row>
     <row r="78">
@@ -1372,11 +1372,11 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79">
@@ -1385,11 +1385,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>in</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>43</v>
+        <v>72</v>
       </c>
     </row>
     <row r="80">
@@ -1398,7 +1398,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>tmp_list_origin</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1411,11 +1411,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>:</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="82">
@@ -1424,11 +1424,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>tmp_list_dict</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="83">
@@ -1437,11 +1437,11 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84">
@@ -1450,11 +1450,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>append</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>46</v>
+        <v>81</v>
       </c>
     </row>
     <row r="85">
@@ -1463,11 +1463,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>81</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86">
@@ -1476,11 +1476,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>{</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>35</v>
+        <v>65</v>
       </c>
     </row>
     <row r="87">
@@ -1489,11 +1489,11 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88">
@@ -1502,11 +1502,11 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>:</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="89">
@@ -1515,23 +1515,24 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>self</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>81</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="n">
         <v>88</v>
       </c>
-      <c r="B90">
-        <f>=</f>
-        <v/>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
       </c>
       <c r="C90" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="91">
@@ -1540,7 +1541,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>b</t>
+          <t>__getWordCode</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1553,11 +1554,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>:</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="93">
@@ -1566,7 +1567,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>word</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1579,11 +1580,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="95">
@@ -1592,11 +1593,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>}</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="96">
@@ -1605,11 +1606,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>17</v>
+        <v>62</v>
       </c>
     </row>
     <row r="97">
@@ -1618,7 +1619,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>word_code_list</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1629,12 +1630,13 @@
       <c r="A98" s="1" t="n">
         <v>96</v>
       </c>
-      <c r="B98">
-        <f>=</f>
-        <v/>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>.</t>
+        </is>
       </c>
       <c r="C98" t="n">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99">
@@ -1643,7 +1645,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>extend</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -1656,11 +1658,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>:</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>33</v>
+        <v>61</v>
       </c>
     </row>
     <row r="101">
@@ -1669,11 +1671,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>if</t>
+          <t>tmp_list_dict</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>17</v>
+        <v>81</v>
       </c>
     </row>
     <row r="102">
@@ -1682,11 +1684,11 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="103">
@@ -1695,11 +1697,11 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>&gt;=</t>
+          <t>self</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>49</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104">
@@ -1708,11 +1710,11 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>.</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>80</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105">
@@ -1721,11 +1723,11 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>:</t>
+          <t>__storeResultsInExcel</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>33</v>
+        <v>81</v>
       </c>
     </row>
     <row r="106">
@@ -1734,11 +1736,11 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t xml:space="preserve">	while</t>
+          <t>(</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>-1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="107">
@@ -1747,11 +1749,11 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>True</t>
+          <t>word_code_list</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="108">
@@ -1760,11 +1762,11 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>#</t>
+          <t>)</t>
         </is>
       </c>
       <c r="C108" t="n">
-        <v>43</v>
+        <v>62</v>
       </c>
     </row>
     <row r="109">
@@ -1773,11 +1775,11 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>a</t>
+          <t>return</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>81</v>
+        <v>27</v>
       </c>
     </row>
     <row r="110">
@@ -1786,24 +1788,11 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>=</t>
+          <t>word_code_list</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="n">
-        <v>109</v>
-      </c>
-      <c r="B111" t="inlineStr">
-        <is>
-          <t>100</t>
-        </is>
-      </c>
-      <c r="C111" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>